<commit_message>
Import & export of xlsx, docx files implemented
</commit_message>
<xml_diff>
--- a/DbBicyclesLab/TableIn.xlsx
+++ b/DbBicyclesLab/TableIn.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Stella 6.1" sheetId="2" r:id="rId1"/>
+    <sheet name="Stella" sheetId="2" r:id="rId1"/>
     <sheet name="TRAIL Neo 3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Розмір</t>
   </si>
@@ -34,7 +34,19 @@
     <t>Q</t>
   </si>
   <si>
-    <t>S</t>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -383,6 +395,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
@@ -402,39 +451,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>123</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>